<commit_message>
update names of variables in core dataset
</commit_message>
<xml_diff>
--- a/field_names_categorization.xlsx
+++ b/field_names_categorization.xlsx
@@ -182,15 +182,15 @@
     <t>A private rental market apartment with no rental subsidy</t>
   </si>
   <si>
+    <t>City-financed homeless set-aside units units financed jointly by HPD and HDC under Housing New York</t>
+  </si>
+  <si>
     <t>City-financed homeless set-aside units- HDC set- aside units financed under Housing New York</t>
   </si>
   <si>
     <t>City-financed homeless set-aside units- HPD set-aside units financed under Housing New York</t>
   </si>
   <si>
-    <t>City-financed homeless set-aside units units financed jointly by HPD and HDC under Housing New York</t>
-  </si>
-  <si>
     <t>CityFHEPS (Family Homelessness and Eviction Prevention Supplement)</t>
   </si>
   <si>
@@ -245,97 +245,97 @@
     <t>Private housing that is not an entire apartment with a rental subsidy- unsubsidized single-room occupancy that is not supportive housing</t>
   </si>
   <si>
+    <t>Private rental market apartment with a rental subsidy- disaggregated by the type of such subsidy (CFHEPS)</t>
+  </si>
+  <si>
+    <t>Private rental market apartment with a rental subsidy- disaggregated by the type of such subsidy (EHV)</t>
+  </si>
+  <si>
+    <t>Private rental market apartment with a rental subsidy- disaggregated by the type of such subsidy (FHEPS)</t>
+  </si>
+  <si>
+    <t>Private rental market apartment with a rental subsidy- disaggregated by the type of such subsidy (SOTA)</t>
+  </si>
+  <si>
+    <t>Private rental market apartment with a rental subsidy- disaggregated by the type of such subsidy (other_sub_exit)</t>
+  </si>
+  <si>
+    <t>Rapid re-housing funded by the United States department of housing and urban development</t>
+  </si>
+  <si>
+    <t>Residential drug treatment and detoxification</t>
+  </si>
+  <si>
+    <t>Section 8</t>
+  </si>
+  <si>
+    <t>Section 8 voucher housing- HPD- project-based</t>
+  </si>
+  <si>
+    <t>Section 8 voucher housing- HPD- tenant-based</t>
+  </si>
+  <si>
+    <t>Section 8 voucher housing- NYC Housing Authority (NYCHA)- project-based</t>
+  </si>
+  <si>
+    <t>Section 8 voucher housing- NYCHA- project-based</t>
+  </si>
+  <si>
+    <t>Section 8 voucher housing- NYCHA- tenant-based</t>
+  </si>
+  <si>
+    <t>Section 8 voucher housing- New York state homes and community renewal- tenant-based</t>
+  </si>
+  <si>
+    <t>Section 8 voucher housing- New York state homes and community renewal-project-based</t>
+  </si>
+  <si>
+    <t>Settings with higher levels of medical care- inpatient hospitalization</t>
+  </si>
+  <si>
+    <t>Settings with higher levels of medical care- long-term care facilities</t>
+  </si>
+  <si>
+    <t>Settings with higher levels of medical care- medical rehabilitation centers</t>
+  </si>
+  <si>
+    <t>Settings with higher levels of medical care- medical respite care</t>
+  </si>
+  <si>
+    <t>Shared Living (Not friends or relatives)</t>
+  </si>
+  <si>
+    <t>Subsidized Apartment (NYCHA, Mitchell Lama, Etc.)</t>
+  </si>
+  <si>
+    <t>Supportive housing</t>
+  </si>
+  <si>
+    <t>Transitional housing operated by or under contract or similar agreement with DHS, DYCD, HPD, United States Department of Housing and Urban Development (HUD) or HRA</t>
+  </si>
+  <si>
+    <t>Transitional housing operated by or under contract or similar agreement with DHS, DYCD, HPD, United States department of housing and urban development or HRA</t>
+  </si>
+  <si>
+    <t>Unknown or unable to validate</t>
+  </si>
+  <si>
+    <t>Youth detention center/Correctional facility</t>
+  </si>
+  <si>
     <t>private rental market apartment with a rental subsidy- disaggregated by the type of such subsidy</t>
   </si>
   <si>
-    <t>Private rental market apartment with a rental subsidy- disaggregated by the type of such subsidy (CFHEPS)</t>
-  </si>
-  <si>
-    <t>Private rental market apartment with a rental subsidy- disaggregated by the type of such subsidy (EHV)</t>
-  </si>
-  <si>
-    <t>Private rental market apartment with a rental subsidy- disaggregated by the type of such subsidy (FHEPS)</t>
-  </si>
-  <si>
-    <t>Private rental market apartment with a rental subsidy- disaggregated by the type of such subsidy (other_sub_exit)</t>
-  </si>
-  <si>
-    <t>Private rental market apartment with a rental subsidy- disaggregated by the type of such subsidy (SOTA)</t>
-  </si>
-  <si>
-    <t>Rapid re-housing funded by the United States department of housing and urban development</t>
-  </si>
-  <si>
-    <t>Residential drug treatment and detoxification</t>
-  </si>
-  <si>
-    <t>Section 8</t>
-  </si>
-  <si>
-    <t>Section 8 voucher housing- HPD- project-based</t>
-  </si>
-  <si>
-    <t>Section 8 voucher housing- HPD- tenant-based</t>
-  </si>
-  <si>
-    <t>Section 8 voucher housing- New York state homes and community renewal- tenant-based</t>
-  </si>
-  <si>
-    <t>Section 8 voucher housing- New York state homes and community renewal-project-based</t>
-  </si>
-  <si>
-    <t>Section 8 voucher housing- NYC Housing Authority (NYCHA)- project-based</t>
-  </si>
-  <si>
-    <t>Section 8 voucher housing- NYCHA- project-based</t>
-  </si>
-  <si>
-    <t>Section 8 voucher housing- NYCHA- tenant-based</t>
-  </si>
-  <si>
     <t>settings with higher levels of medical care- inpatient hospitalization</t>
   </si>
   <si>
-    <t>Settings with higher levels of medical care- inpatient hospitalization</t>
-  </si>
-  <si>
     <t>settings with higher levels of medical care- long-term care facilities</t>
   </si>
   <si>
-    <t>Settings with higher levels of medical care- long-term care facilities</t>
-  </si>
-  <si>
     <t>settings with higher levels of medical care- medical rehabilitation centers</t>
   </si>
   <si>
-    <t>Settings with higher levels of medical care- medical rehabilitation centers</t>
-  </si>
-  <si>
     <t>settings with higher levels of medical care- medical respite care</t>
-  </si>
-  <si>
-    <t>Settings with higher levels of medical care- medical respite care</t>
-  </si>
-  <si>
-    <t>Shared Living (Not friends or relatives)</t>
-  </si>
-  <si>
-    <t>Subsidized Apartment (NYCHA, Mitchell Lama, Etc.)</t>
-  </si>
-  <si>
-    <t>Supportive housing</t>
-  </si>
-  <si>
-    <t>Transitional housing operated by or under contract or similar agreement with DHS, DYCD, HPD, United States Department of Housing and Urban Development (HUD) or HRA</t>
-  </si>
-  <si>
-    <t>Transitional housing operated by or under contract or similar agreement with DHS, DYCD, HPD, United States department of housing and urban development or HRA</t>
-  </si>
-  <si>
-    <t>Unknown or unable to validate</t>
-  </si>
-  <si>
-    <t>Youth detention center/Correctional facility</t>
   </si>
 </sst>
 </file>
@@ -645,7 +645,7 @@
         <v>77</v>
       </c>
       <c r="C24" t="n">
-        <v>21.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="25">
@@ -700,7 +700,7 @@
         <v>82</v>
       </c>
       <c r="C29" t="n">
-        <v>7.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="30">
@@ -722,7 +722,7 @@
         <v>84</v>
       </c>
       <c r="C31" t="n">
-        <v>28.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="32">
@@ -733,7 +733,7 @@
         <v>85</v>
       </c>
       <c r="C32" t="n">
-        <v>14.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="33">
@@ -755,7 +755,7 @@
         <v>87</v>
       </c>
       <c r="C34" t="n">
-        <v>28.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="35">
@@ -766,7 +766,7 @@
         <v>88</v>
       </c>
       <c r="C35" t="n">
-        <v>28.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="36">
@@ -788,7 +788,7 @@
         <v>90</v>
       </c>
       <c r="C37" t="n">
-        <v>21.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="38">
@@ -799,7 +799,7 @@
         <v>91</v>
       </c>
       <c r="C38" t="n">
-        <v>7.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="39">
@@ -810,7 +810,7 @@
         <v>92</v>
       </c>
       <c r="C39" t="n">
-        <v>28.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="40">
@@ -821,7 +821,7 @@
         <v>93</v>
       </c>
       <c r="C40" t="n">
-        <v>7.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="41">
@@ -843,7 +843,7 @@
         <v>95</v>
       </c>
       <c r="C42" t="n">
-        <v>7.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="43">
@@ -854,7 +854,7 @@
         <v>96</v>
       </c>
       <c r="C43" t="n">
-        <v>21.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="44">
@@ -876,7 +876,7 @@
         <v>98</v>
       </c>
       <c r="C45" t="n">
-        <v>21.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="46">
@@ -887,7 +887,7 @@
         <v>99</v>
       </c>
       <c r="C46" t="n">
-        <v>7.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="47">
@@ -898,7 +898,7 @@
         <v>100</v>
       </c>
       <c r="C47" t="n">
-        <v>21.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="48">
@@ -909,7 +909,7 @@
         <v>101</v>
       </c>
       <c r="C48" t="n">
-        <v>7.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="49">
@@ -931,7 +931,7 @@
         <v>103</v>
       </c>
       <c r="C50" t="n">
-        <v>28.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="51">
@@ -942,7 +942,7 @@
         <v>104</v>
       </c>
       <c r="C51" t="n">
-        <v>21.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="52">
@@ -964,7 +964,7 @@
         <v>106</v>
       </c>
       <c r="C53" t="n">
-        <v>28.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="54">

</xml_diff>

<commit_message>
update analysis with december report data
</commit_message>
<xml_diff>
--- a/field_names_categorization.xlsx
+++ b/field_names_categorization.xlsx
@@ -403,7 +403,7 @@
         <v>55</v>
       </c>
       <c r="C2" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="3">
@@ -414,7 +414,7 @@
         <v>56</v>
       </c>
       <c r="C3" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="4">
@@ -425,7 +425,7 @@
         <v>57</v>
       </c>
       <c r="C4" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="5">
@@ -436,7 +436,7 @@
         <v>58</v>
       </c>
       <c r="C5" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="6">
@@ -447,7 +447,7 @@
         <v>59</v>
       </c>
       <c r="C6" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="7">
@@ -458,7 +458,7 @@
         <v>60</v>
       </c>
       <c r="C7" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="8">
@@ -469,7 +469,7 @@
         <v>61</v>
       </c>
       <c r="C8" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="9">
@@ -480,7 +480,7 @@
         <v>62</v>
       </c>
       <c r="C9" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="10">
@@ -491,7 +491,7 @@
         <v>63</v>
       </c>
       <c r="C10" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="11">
@@ -502,7 +502,7 @@
         <v>64</v>
       </c>
       <c r="C11" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="12">
@@ -513,7 +513,7 @@
         <v>65</v>
       </c>
       <c r="C12" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="13">
@@ -524,7 +524,7 @@
         <v>66</v>
       </c>
       <c r="C13" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="14">
@@ -535,7 +535,7 @@
         <v>67</v>
       </c>
       <c r="C14" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="15">
@@ -546,7 +546,7 @@
         <v>68</v>
       </c>
       <c r="C15" t="n">
-        <v>14.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="16">
@@ -557,7 +557,7 @@
         <v>69</v>
       </c>
       <c r="C16" t="n">
-        <v>14.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="17">
@@ -568,7 +568,7 @@
         <v>70</v>
       </c>
       <c r="C17" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="18">
@@ -579,7 +579,7 @@
         <v>71</v>
       </c>
       <c r="C18" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="19">
@@ -590,7 +590,7 @@
         <v>72</v>
       </c>
       <c r="C19" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="20">
@@ -601,7 +601,7 @@
         <v>73</v>
       </c>
       <c r="C20" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="21">
@@ -612,7 +612,7 @@
         <v>74</v>
       </c>
       <c r="C21" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="22">
@@ -623,7 +623,7 @@
         <v>75</v>
       </c>
       <c r="C22" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="23">
@@ -634,7 +634,7 @@
         <v>76</v>
       </c>
       <c r="C23" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="24">
@@ -645,7 +645,7 @@
         <v>77</v>
       </c>
       <c r="C24" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="25">
@@ -656,7 +656,7 @@
         <v>78</v>
       </c>
       <c r="C25" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="26">
@@ -667,7 +667,7 @@
         <v>79</v>
       </c>
       <c r="C26" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="27">
@@ -678,7 +678,7 @@
         <v>80</v>
       </c>
       <c r="C27" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="28">
@@ -689,7 +689,7 @@
         <v>81</v>
       </c>
       <c r="C28" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="29">
@@ -700,7 +700,7 @@
         <v>82</v>
       </c>
       <c r="C29" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="30">
@@ -711,7 +711,7 @@
         <v>83</v>
       </c>
       <c r="C30" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="31">
@@ -722,7 +722,7 @@
         <v>84</v>
       </c>
       <c r="C31" t="n">
-        <v>14.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="32">
@@ -733,7 +733,7 @@
         <v>85</v>
       </c>
       <c r="C32" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="33">
@@ -744,7 +744,7 @@
         <v>86</v>
       </c>
       <c r="C33" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="34">
@@ -755,7 +755,7 @@
         <v>87</v>
       </c>
       <c r="C34" t="n">
-        <v>21.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="35">
@@ -766,7 +766,7 @@
         <v>88</v>
       </c>
       <c r="C35" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="36">
@@ -777,7 +777,7 @@
         <v>89</v>
       </c>
       <c r="C36" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="37">
@@ -788,7 +788,7 @@
         <v>90</v>
       </c>
       <c r="C37" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="38">
@@ -799,7 +799,7 @@
         <v>91</v>
       </c>
       <c r="C38" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="39">
@@ -810,7 +810,7 @@
         <v>92</v>
       </c>
       <c r="C39" t="n">
-        <v>21.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="40">
@@ -821,7 +821,7 @@
         <v>93</v>
       </c>
       <c r="C40" t="n">
-        <v>21.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="41">
@@ -832,7 +832,7 @@
         <v>94</v>
       </c>
       <c r="C41" t="n">
-        <v>21.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="42">
@@ -843,7 +843,7 @@
         <v>95</v>
       </c>
       <c r="C42" t="n">
-        <v>21.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="43">
@@ -854,7 +854,7 @@
         <v>96</v>
       </c>
       <c r="C43" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="44">
@@ -865,7 +865,7 @@
         <v>97</v>
       </c>
       <c r="C44" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="45">
@@ -876,7 +876,7 @@
         <v>98</v>
       </c>
       <c r="C45" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="46">
@@ -887,7 +887,7 @@
         <v>99</v>
       </c>
       <c r="C46" t="n">
-        <v>21.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="47">
@@ -898,7 +898,7 @@
         <v>100</v>
       </c>
       <c r="C47" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="48">
@@ -909,7 +909,7 @@
         <v>101</v>
       </c>
       <c r="C48" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="49">
@@ -920,7 +920,7 @@
         <v>102</v>
       </c>
       <c r="C49" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="50">
@@ -931,7 +931,7 @@
         <v>103</v>
       </c>
       <c r="C50" t="n">
-        <v>21.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="51">
@@ -942,7 +942,7 @@
         <v>104</v>
       </c>
       <c r="C51" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="52">
@@ -953,7 +953,7 @@
         <v>105</v>
       </c>
       <c r="C52" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="53">
@@ -964,7 +964,7 @@
         <v>106</v>
       </c>
       <c r="C53" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="54">
@@ -975,7 +975,7 @@
         <v>107</v>
       </c>
       <c r="C54" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with jan data
</commit_message>
<xml_diff>
--- a/field_names_categorization.xlsx
+++ b/field_names_categorization.xlsx
@@ -403,7 +403,7 @@
         <v>55</v>
       </c>
       <c r="C2" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="3">
@@ -414,7 +414,7 @@
         <v>56</v>
       </c>
       <c r="C3" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="4">
@@ -425,7 +425,7 @@
         <v>57</v>
       </c>
       <c r="C4" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="5">
@@ -436,7 +436,7 @@
         <v>58</v>
       </c>
       <c r="C5" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="6">
@@ -447,7 +447,7 @@
         <v>59</v>
       </c>
       <c r="C6" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="7">
@@ -458,7 +458,7 @@
         <v>60</v>
       </c>
       <c r="C7" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="8">
@@ -469,7 +469,7 @@
         <v>61</v>
       </c>
       <c r="C8" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="9">
@@ -480,7 +480,7 @@
         <v>62</v>
       </c>
       <c r="C9" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="10">
@@ -491,7 +491,7 @@
         <v>63</v>
       </c>
       <c r="C10" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="11">
@@ -502,7 +502,7 @@
         <v>64</v>
       </c>
       <c r="C11" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="12">
@@ -513,7 +513,7 @@
         <v>65</v>
       </c>
       <c r="C12" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="13">
@@ -524,7 +524,7 @@
         <v>66</v>
       </c>
       <c r="C13" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="14">
@@ -535,7 +535,7 @@
         <v>67</v>
       </c>
       <c r="C14" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="15">
@@ -546,7 +546,7 @@
         <v>68</v>
       </c>
       <c r="C15" t="n">
-        <v>16.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="16">
@@ -557,7 +557,7 @@
         <v>69</v>
       </c>
       <c r="C16" t="n">
-        <v>16.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="17">
@@ -568,7 +568,7 @@
         <v>70</v>
       </c>
       <c r="C17" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="18">
@@ -579,7 +579,7 @@
         <v>71</v>
       </c>
       <c r="C18" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="19">
@@ -590,7 +590,7 @@
         <v>72</v>
       </c>
       <c r="C19" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="20">
@@ -601,7 +601,7 @@
         <v>73</v>
       </c>
       <c r="C20" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="21">
@@ -612,7 +612,7 @@
         <v>74</v>
       </c>
       <c r="C21" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="22">
@@ -623,7 +623,7 @@
         <v>75</v>
       </c>
       <c r="C22" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="23">
@@ -634,7 +634,7 @@
         <v>76</v>
       </c>
       <c r="C23" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="24">
@@ -645,7 +645,7 @@
         <v>77</v>
       </c>
       <c r="C24" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="25">
@@ -656,7 +656,7 @@
         <v>78</v>
       </c>
       <c r="C25" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="26">
@@ -667,7 +667,7 @@
         <v>79</v>
       </c>
       <c r="C26" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="27">
@@ -678,7 +678,7 @@
         <v>80</v>
       </c>
       <c r="C27" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="28">
@@ -689,7 +689,7 @@
         <v>81</v>
       </c>
       <c r="C28" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="29">
@@ -700,7 +700,7 @@
         <v>82</v>
       </c>
       <c r="C29" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="30">
@@ -711,7 +711,7 @@
         <v>83</v>
       </c>
       <c r="C30" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="31">
@@ -722,7 +722,7 @@
         <v>84</v>
       </c>
       <c r="C31" t="n">
-        <v>16.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="32">
@@ -733,7 +733,7 @@
         <v>85</v>
       </c>
       <c r="C32" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="33">
@@ -744,7 +744,7 @@
         <v>86</v>
       </c>
       <c r="C33" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="34">
@@ -755,7 +755,7 @@
         <v>87</v>
       </c>
       <c r="C34" t="n">
-        <v>24.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="35">
@@ -766,7 +766,7 @@
         <v>88</v>
       </c>
       <c r="C35" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="36">
@@ -777,7 +777,7 @@
         <v>89</v>
       </c>
       <c r="C36" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="37">
@@ -788,7 +788,7 @@
         <v>90</v>
       </c>
       <c r="C37" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="38">
@@ -799,7 +799,7 @@
         <v>91</v>
       </c>
       <c r="C38" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="39">
@@ -810,7 +810,7 @@
         <v>92</v>
       </c>
       <c r="C39" t="n">
-        <v>24.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="40">
@@ -821,7 +821,7 @@
         <v>93</v>
       </c>
       <c r="C40" t="n">
-        <v>24.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="41">
@@ -832,7 +832,7 @@
         <v>94</v>
       </c>
       <c r="C41" t="n">
-        <v>24.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="42">
@@ -843,7 +843,7 @@
         <v>95</v>
       </c>
       <c r="C42" t="n">
-        <v>24.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="43">
@@ -854,7 +854,7 @@
         <v>96</v>
       </c>
       <c r="C43" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="44">
@@ -865,7 +865,7 @@
         <v>97</v>
       </c>
       <c r="C44" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="45">
@@ -876,7 +876,7 @@
         <v>98</v>
       </c>
       <c r="C45" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="46">
@@ -887,7 +887,7 @@
         <v>99</v>
       </c>
       <c r="C46" t="n">
-        <v>24.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="47">
@@ -898,7 +898,7 @@
         <v>100</v>
       </c>
       <c r="C47" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="48">
@@ -909,7 +909,7 @@
         <v>101</v>
       </c>
       <c r="C48" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="49">
@@ -920,7 +920,7 @@
         <v>102</v>
       </c>
       <c r="C49" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="50">
@@ -931,7 +931,7 @@
         <v>103</v>
       </c>
       <c r="C50" t="n">
-        <v>24.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="51">
@@ -942,7 +942,7 @@
         <v>104</v>
       </c>
       <c r="C51" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="52">
@@ -953,7 +953,7 @@
         <v>105</v>
       </c>
       <c r="C52" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="53">
@@ -964,7 +964,7 @@
         <v>106</v>
       </c>
       <c r="C53" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="54">
@@ -975,7 +975,7 @@
         <v>107</v>
       </c>
       <c r="C54" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>